<commit_message>
Add figures and notebook for investigating serum+metadata ML features
</commit_message>
<xml_diff>
--- a/tables/ml_model_performance.xlsx
+++ b/tables/ml_model_performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tgroth/Google Drive/knight_twin_NAFLD/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99867AA-784C-F745-A4BA-8C566E1E3D62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA9618A-39D9-F047-A467-712C06D96178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="25820" windowHeight="17400" activeTab="6" xr2:uid="{674D796F-A39C-4A47-8627-A0CC1E2D624E}"/>
+    <workbookView xWindow="1600" yWindow="460" windowWidth="25820" windowHeight="17400" firstSheet="1" activeTab="8" xr2:uid="{674D796F-A39C-4A47-8627-A0CC1E2D624E}"/>
   </bookViews>
   <sheets>
     <sheet name="Serum ScaledFT" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="FullMulti ScaledFT" sheetId="8" r:id="rId6"/>
     <sheet name="SerumMutli ScaledFT" sheetId="9" r:id="rId7"/>
     <sheet name="FecalMutli ScaledFT" sheetId="10" r:id="rId8"/>
+    <sheet name="SerumMeta ScaledFt" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="162">
   <si>
     <t>Metric</t>
   </si>
@@ -551,6 +552,27 @@
   <si>
     <t>Further Selection + Metadata
 (19 Features)</t>
+  </si>
+  <si>
+    <t>Feature Selection + Gender
+(50 Features)</t>
+  </si>
+  <si>
+    <t>0.81 (0), 0.41(1)</t>
+  </si>
+  <si>
+    <t>Feature Selection  + BMI
+(50 Features)</t>
+  </si>
+  <si>
+    <t>0.88 (0), 0.34 (1)</t>
+  </si>
+  <si>
+    <t>Feature Selection + Age
+(50 Features)</t>
+  </si>
+  <si>
+    <t>0.89 (0), 0.70 (1)</t>
   </si>
 </sst>
 </file>
@@ -599,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -653,17 +675,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -984,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B090CD82-F333-604B-88EF-95561D3BFF64}">
   <dimension ref="C3:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -998,13 +1029,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
@@ -1024,10 +1055,10 @@
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1041,8 +1072,8 @@
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="7" t="s">
         <v>5</v>
       </c>
@@ -1054,8 +1085,8 @@
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C7" s="21"/>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="7" t="s">
@@ -1069,8 +1100,8 @@
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="7" t="s">
         <v>5</v>
       </c>
@@ -1082,10 +1113,10 @@
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -1099,8 +1130,8 @@
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="7" t="s">
         <v>5</v>
       </c>
@@ -1112,8 +1143,8 @@
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C11" s="21"/>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="7" t="s">
@@ -1127,8 +1158,8 @@
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="7" t="s">
         <v>5</v>
       </c>
@@ -1140,10 +1171,10 @@
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -1157,8 +1188,8 @@
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="7" t="s">
         <v>5</v>
       </c>
@@ -1170,8 +1201,8 @@
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C15" s="21"/>
-      <c r="D15" s="20" t="s">
+      <c r="C15" s="22"/>
+      <c r="D15" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="7" t="s">
@@ -1185,8 +1216,8 @@
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
       <c r="E16" s="7" t="s">
         <v>5</v>
       </c>
@@ -1198,10 +1229,10 @@
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -1215,8 +1246,8 @@
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="7" t="s">
         <v>5</v>
       </c>
@@ -1228,8 +1259,8 @@
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C19" s="21"/>
-      <c r="D19" s="20" t="s">
+      <c r="C19" s="22"/>
+      <c r="D19" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -1243,8 +1274,8 @@
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="7" t="s">
         <v>5</v>
       </c>
@@ -1256,10 +1287,10 @@
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="7" t="s">
@@ -1273,8 +1304,8 @@
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
       <c r="E22" s="7" t="s">
         <v>5</v>
       </c>
@@ -1286,8 +1317,8 @@
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C23" s="21"/>
-      <c r="D23" s="20" t="s">
+      <c r="C23" s="22"/>
+      <c r="D23" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="7" t="s">
@@ -1301,8 +1332,8 @@
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="7" t="s">
         <v>5</v>
       </c>
@@ -1314,10 +1345,10 @@
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="7" t="s">
@@ -1331,8 +1362,8 @@
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="7" t="s">
         <v>5</v>
       </c>
@@ -1344,8 +1375,8 @@
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C27" s="21"/>
-      <c r="D27" s="20" t="s">
+      <c r="C27" s="22"/>
+      <c r="D27" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -1359,8 +1390,8 @@
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="7" t="s">
         <v>5</v>
       </c>
@@ -1372,10 +1403,10 @@
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -1389,8 +1420,8 @@
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="7" t="s">
         <v>5</v>
       </c>
@@ -1402,8 +1433,8 @@
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C31" s="21"/>
-      <c r="D31" s="20" t="s">
+      <c r="C31" s="22"/>
+      <c r="D31" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -1417,8 +1448,8 @@
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="7" t="s">
         <v>5</v>
       </c>
@@ -1430,10 +1461,10 @@
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="7" t="s">
@@ -1447,8 +1478,8 @@
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="7" t="s">
         <v>5</v>
       </c>
@@ -1460,8 +1491,8 @@
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C35" s="21"/>
-      <c r="D35" s="20" t="s">
+      <c r="C35" s="22"/>
+      <c r="D35" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="7" t="s">
@@ -1475,8 +1506,8 @@
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
       <c r="E36" s="7" t="s">
         <v>5</v>
       </c>
@@ -1488,10 +1519,10 @@
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E37" s="7" t="s">
@@ -1505,8 +1536,8 @@
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
       <c r="E38" s="7" t="s">
         <v>5</v>
       </c>
@@ -1518,8 +1549,8 @@
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C39" s="21"/>
-      <c r="D39" s="20" t="s">
+      <c r="C39" s="22"/>
+      <c r="D39" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E39" s="7" t="s">
@@ -1533,8 +1564,8 @@
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
       <c r="E40" s="7" t="s">
         <v>5</v>
       </c>
@@ -1546,10 +1577,10 @@
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="7" t="s">
@@ -1563,8 +1594,8 @@
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
       <c r="E42" s="7" t="s">
         <v>5</v>
       </c>
@@ -1576,8 +1607,8 @@
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C43" s="21"/>
-      <c r="D43" s="20" t="s">
+      <c r="C43" s="22"/>
+      <c r="D43" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E43" s="7" t="s">
@@ -1591,8 +1622,8 @@
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="7" t="s">
         <v>5</v>
       </c>
@@ -1605,21 +1636,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C41:C44"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D31:D32"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="D25:D26"/>
@@ -1636,6 +1652,21 @@
     <mergeCell ref="C17:C20"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C41:C44"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D39:D40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1659,13 +1690,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
@@ -1685,10 +1716,10 @@
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -1702,8 +1733,8 @@
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="7" t="s">
         <v>5</v>
       </c>
@@ -1715,8 +1746,8 @@
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C7" s="21"/>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="7" t="s">
@@ -1730,8 +1761,8 @@
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="7" t="s">
         <v>5</v>
       </c>
@@ -1743,10 +1774,10 @@
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -1760,8 +1791,8 @@
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="7" t="s">
         <v>5</v>
       </c>
@@ -1773,8 +1804,8 @@
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C11" s="21"/>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="7" t="s">
@@ -1788,8 +1819,8 @@
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="7" t="s">
         <v>5</v>
       </c>
@@ -1801,10 +1832,10 @@
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -1818,8 +1849,8 @@
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="7" t="s">
         <v>5</v>
       </c>
@@ -1831,8 +1862,8 @@
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C15" s="21"/>
-      <c r="D15" s="20" t="s">
+      <c r="C15" s="22"/>
+      <c r="D15" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="7" t="s">
@@ -1846,8 +1877,8 @@
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
       <c r="E16" s="7" t="s">
         <v>5</v>
       </c>
@@ -1859,10 +1890,10 @@
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -1876,8 +1907,8 @@
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="7" t="s">
         <v>5</v>
       </c>
@@ -1889,8 +1920,8 @@
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C19" s="21"/>
-      <c r="D19" s="20" t="s">
+      <c r="C19" s="22"/>
+      <c r="D19" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -1904,8 +1935,8 @@
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="7" t="s">
         <v>5</v>
       </c>
@@ -1917,10 +1948,10 @@
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="7" t="s">
@@ -1934,8 +1965,8 @@
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
       <c r="E22" s="7" t="s">
         <v>5</v>
       </c>
@@ -1947,8 +1978,8 @@
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C23" s="21"/>
-      <c r="D23" s="20" t="s">
+      <c r="C23" s="22"/>
+      <c r="D23" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="7" t="s">
@@ -1962,8 +1993,8 @@
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="7" t="s">
         <v>5</v>
       </c>
@@ -1975,10 +2006,10 @@
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="7" t="s">
@@ -1992,8 +2023,8 @@
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="7" t="s">
         <v>5</v>
       </c>
@@ -2005,8 +2036,8 @@
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C27" s="21"/>
-      <c r="D27" s="20" t="s">
+      <c r="C27" s="22"/>
+      <c r="D27" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -2020,8 +2051,8 @@
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="7" t="s">
         <v>5</v>
       </c>
@@ -2033,10 +2064,10 @@
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -2050,8 +2081,8 @@
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="7" t="s">
         <v>5</v>
       </c>
@@ -2063,8 +2094,8 @@
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C31" s="21"/>
-      <c r="D31" s="20" t="s">
+      <c r="C31" s="22"/>
+      <c r="D31" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -2078,8 +2109,8 @@
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="7" t="s">
         <v>5</v>
       </c>
@@ -2091,10 +2122,10 @@
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="7" t="s">
@@ -2108,8 +2139,8 @@
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="7" t="s">
         <v>5</v>
       </c>
@@ -2121,8 +2152,8 @@
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C35" s="21"/>
-      <c r="D35" s="20" t="s">
+      <c r="C35" s="22"/>
+      <c r="D35" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="7" t="s">
@@ -2136,8 +2167,8 @@
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
       <c r="E36" s="7" t="s">
         <v>5</v>
       </c>
@@ -2149,10 +2180,10 @@
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E37" s="7" t="s">
@@ -2166,8 +2197,8 @@
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
       <c r="E38" s="7" t="s">
         <v>5</v>
       </c>
@@ -2179,8 +2210,8 @@
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C39" s="21"/>
-      <c r="D39" s="20" t="s">
+      <c r="C39" s="22"/>
+      <c r="D39" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E39" s="7" t="s">
@@ -2194,8 +2225,8 @@
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
       <c r="E40" s="7" t="s">
         <v>5</v>
       </c>
@@ -2207,10 +2238,10 @@
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="7" t="s">
@@ -2224,8 +2255,8 @@
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
       <c r="E42" s="7" t="s">
         <v>5</v>
       </c>
@@ -2237,8 +2268,8 @@
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C43" s="21"/>
-      <c r="D43" s="20" t="s">
+      <c r="C43" s="22"/>
+      <c r="D43" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E43" s="7" t="s">
@@ -2252,8 +2283,8 @@
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="7" t="s">
         <v>5</v>
       </c>
@@ -2266,6 +2297,25 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
     <mergeCell ref="C29:C32"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="D29:D30"/>
@@ -2278,25 +2328,6 @@
     <mergeCell ref="C37:C40"/>
     <mergeCell ref="D39:D40"/>
     <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2322,13 +2353,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C3" s="2" t="s">
@@ -2348,10 +2379,10 @@
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -2365,8 +2396,8 @@
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
       <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
@@ -2378,8 +2409,8 @@
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C6" s="21"/>
-      <c r="D6" s="20" t="s">
+      <c r="C6" s="22"/>
+      <c r="D6" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -2393,8 +2424,8 @@
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2406,10 +2437,10 @@
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -2423,8 +2454,8 @@
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="5" t="s">
         <v>5</v>
       </c>
@@ -2436,8 +2467,8 @@
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C10" s="21"/>
-      <c r="D10" s="20" t="s">
+      <c r="C10" s="22"/>
+      <c r="D10" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -2451,8 +2482,8 @@
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="5" t="s">
         <v>5</v>
       </c>
@@ -2464,10 +2495,10 @@
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="26" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -2481,8 +2512,8 @@
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C13" s="21"/>
-      <c r="D13" s="19"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="5" t="s">
         <v>5</v>
       </c>
@@ -2494,8 +2525,8 @@
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C14" s="21"/>
-      <c r="D14" s="23" t="s">
+      <c r="C14" s="22"/>
+      <c r="D14" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -2509,8 +2540,8 @@
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C15" s="21"/>
-      <c r="D15" s="19"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="25"/>
       <c r="E15" s="5" t="s">
         <v>5</v>
       </c>
@@ -2522,10 +2553,10 @@
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -2539,8 +2570,8 @@
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
       <c r="E17" s="5" t="s">
         <v>5</v>
       </c>
@@ -2552,8 +2583,8 @@
       </c>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C18" s="21"/>
-      <c r="D18" s="20" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -2567,8 +2598,8 @@
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="5" t="s">
         <v>5</v>
       </c>
@@ -2580,10 +2611,10 @@
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -2597,8 +2628,8 @@
       </c>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
       <c r="E21" s="5" t="s">
         <v>5</v>
       </c>
@@ -2610,8 +2641,8 @@
       </c>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C22" s="21"/>
-      <c r="D22" s="20" t="s">
+      <c r="C22" s="22"/>
+      <c r="D22" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -2625,8 +2656,8 @@
       </c>
     </row>
     <row r="23" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2638,10 +2669,10 @@
       </c>
     </row>
     <row r="24" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -2655,8 +2686,8 @@
       </c>
     </row>
     <row r="25" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
       <c r="E25" s="5" t="s">
         <v>5</v>
       </c>
@@ -2668,8 +2699,8 @@
       </c>
     </row>
     <row r="26" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C26" s="21"/>
-      <c r="D26" s="20" t="s">
+      <c r="C26" s="22"/>
+      <c r="D26" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -2683,8 +2714,8 @@
       </c>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="5" t="s">
         <v>5</v>
       </c>
@@ -2696,10 +2727,10 @@
       </c>
     </row>
     <row r="28" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="10" t="s">
@@ -2711,15 +2742,15 @@
       <c r="G28" s="10">
         <v>0.64</v>
       </c>
-      <c r="I28" s="22"/>
-      <c r="J28" s="20"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="23"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
     <row r="29" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
       <c r="E29" s="10" t="s">
         <v>5</v>
       </c>
@@ -2729,15 +2760,15 @@
       <c r="G29" s="10">
         <v>0.61</v>
       </c>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
       <c r="K29" s="6"/>
       <c r="L29" s="4"/>
       <c r="M29" s="6"/>
     </row>
     <row r="30" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C30" s="21"/>
-      <c r="D30" s="20" t="s">
+      <c r="C30" s="22"/>
+      <c r="D30" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="10" t="s">
@@ -2749,15 +2780,15 @@
       <c r="G30" s="4">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I30" s="21"/>
-      <c r="J30" s="20"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="23"/>
       <c r="K30" s="6"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
     <row r="31" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
       <c r="E31" s="10" t="s">
         <v>5</v>
       </c>
@@ -2767,17 +2798,17 @@
       <c r="G31" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
     </row>
     <row r="32" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="10" t="s">
@@ -2789,15 +2820,15 @@
       <c r="G32" s="10">
         <v>0.87</v>
       </c>
-      <c r="I32" s="22"/>
-      <c r="J32" s="20"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="23"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="10" t="s">
         <v>5</v>
       </c>
@@ -2807,15 +2838,15 @@
       <c r="G33" s="10">
         <v>0.76</v>
       </c>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C34" s="21"/>
-      <c r="D34" s="20" t="s">
+      <c r="C34" s="22"/>
+      <c r="D34" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E34" s="10" t="s">
@@ -2827,15 +2858,15 @@
       <c r="G34" s="10">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="20"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="23"/>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
     </row>
     <row r="35" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
       <c r="E35" s="10" t="s">
         <v>5</v>
       </c>
@@ -2845,17 +2876,17 @@
       <c r="G35" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D36" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E36" s="9" t="s">
@@ -2867,15 +2898,15 @@
       <c r="G36" s="9">
         <v>0.84</v>
       </c>
-      <c r="I36" s="22"/>
-      <c r="J36" s="20"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="23"/>
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
       <c r="E37" s="9" t="s">
         <v>5</v>
       </c>
@@ -2885,15 +2916,15 @@
       <c r="G37" s="9">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C38" s="21"/>
-      <c r="D38" s="20" t="s">
+      <c r="C38" s="22"/>
+      <c r="D38" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E38" s="9" t="s">
@@ -2905,15 +2936,15 @@
       <c r="G38" s="9">
         <v>0.59</v>
       </c>
-      <c r="I38" s="21"/>
-      <c r="J38" s="20"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="23"/>
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
       <c r="M38" s="7"/>
     </row>
     <row r="39" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
       <c r="E39" s="9" t="s">
         <v>5</v>
       </c>
@@ -2923,17 +2954,17 @@
       <c r="G39" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E40" s="7" t="s">
@@ -2945,15 +2976,15 @@
       <c r="G40" s="11">
         <v>0.85</v>
       </c>
-      <c r="I40" s="22"/>
-      <c r="J40" s="20"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="23"/>
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
     </row>
     <row r="41" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
       <c r="E41" s="7" t="s">
         <v>5</v>
       </c>
@@ -2963,15 +2994,15 @@
       <c r="G41" s="11">
         <v>0.85</v>
       </c>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
       <c r="K41" s="6"/>
       <c r="L41" s="4"/>
       <c r="M41" s="6"/>
     </row>
     <row r="42" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C42" s="21"/>
-      <c r="D42" s="20" t="s">
+      <c r="C42" s="22"/>
+      <c r="D42" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E42" s="7" t="s">
@@ -2983,15 +3014,15 @@
       <c r="G42" s="4">
         <v>0.79</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="20"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="23"/>
       <c r="K42" s="6"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
     </row>
     <row r="43" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
       <c r="E43" s="7" t="s">
         <v>5</v>
       </c>
@@ -3001,38 +3032,26 @@
       <c r="G43" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="J34:J35"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="C4:C7"/>
@@ -3040,18 +3059,30 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="D10:D11"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="J40:J41"/>
-    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D36:D37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3075,13 +3106,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="3" t="s">
@@ -3101,10 +3132,10 @@
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -3118,8 +3149,8 @@
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="7" t="s">
         <v>5</v>
       </c>
@@ -3131,8 +3162,8 @@
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C7" s="21"/>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="7" t="s">
@@ -3146,8 +3177,8 @@
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="7" t="s">
         <v>5</v>
       </c>
@@ -3159,10 +3190,10 @@
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -3176,8 +3207,8 @@
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="7" t="s">
         <v>5</v>
       </c>
@@ -3189,8 +3220,8 @@
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C11" s="21"/>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="7" t="s">
@@ -3204,8 +3235,8 @@
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="7" t="s">
         <v>5</v>
       </c>
@@ -3217,10 +3248,10 @@
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -3234,8 +3265,8 @@
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="7" t="s">
         <v>5</v>
       </c>
@@ -3247,8 +3278,8 @@
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C15" s="21"/>
-      <c r="D15" s="20" t="s">
+      <c r="C15" s="22"/>
+      <c r="D15" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="7" t="s">
@@ -3262,8 +3293,8 @@
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
       <c r="E16" s="7" t="s">
         <v>5</v>
       </c>
@@ -3275,10 +3306,10 @@
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -3292,8 +3323,8 @@
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="7" t="s">
         <v>5</v>
       </c>
@@ -3305,8 +3336,8 @@
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C19" s="21"/>
-      <c r="D19" s="20" t="s">
+      <c r="C19" s="22"/>
+      <c r="D19" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -3320,8 +3351,8 @@
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="7" t="s">
         <v>5</v>
       </c>
@@ -3333,10 +3364,10 @@
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="7" t="s">
@@ -3350,8 +3381,8 @@
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
       <c r="E22" s="7" t="s">
         <v>5</v>
       </c>
@@ -3363,8 +3394,8 @@
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C23" s="21"/>
-      <c r="D23" s="20" t="s">
+      <c r="C23" s="22"/>
+      <c r="D23" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="7" t="s">
@@ -3378,8 +3409,8 @@
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="7" t="s">
         <v>5</v>
       </c>
@@ -3391,10 +3422,10 @@
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="7" t="s">
@@ -3408,8 +3439,8 @@
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="7" t="s">
         <v>5</v>
       </c>
@@ -3421,8 +3452,8 @@
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C27" s="21"/>
-      <c r="D27" s="20" t="s">
+      <c r="C27" s="22"/>
+      <c r="D27" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -3436,8 +3467,8 @@
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="7" t="s">
         <v>5</v>
       </c>
@@ -3449,10 +3480,10 @@
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -3466,8 +3497,8 @@
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="7" t="s">
         <v>5</v>
       </c>
@@ -3479,8 +3510,8 @@
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C31" s="21"/>
-      <c r="D31" s="20" t="s">
+      <c r="C31" s="22"/>
+      <c r="D31" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -3494,8 +3525,8 @@
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="7" t="s">
         <v>5</v>
       </c>
@@ -3507,10 +3538,10 @@
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="7" t="s">
@@ -3524,8 +3555,8 @@
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="7" t="s">
         <v>5</v>
       </c>
@@ -3537,8 +3568,8 @@
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C35" s="21"/>
-      <c r="D35" s="20" t="s">
+      <c r="C35" s="22"/>
+      <c r="D35" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="7" t="s">
@@ -3552,8 +3583,8 @@
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
       <c r="E36" s="7" t="s">
         <v>5</v>
       </c>
@@ -3565,10 +3596,10 @@
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E37" s="7" t="s">
@@ -3582,8 +3613,8 @@
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
       <c r="E38" s="7" t="s">
         <v>5</v>
       </c>
@@ -3595,8 +3626,8 @@
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C39" s="21"/>
-      <c r="D39" s="20" t="s">
+      <c r="C39" s="22"/>
+      <c r="D39" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E39" s="7" t="s">
@@ -3610,8 +3641,8 @@
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
       <c r="E40" s="7" t="s">
         <v>5</v>
       </c>
@@ -3623,10 +3654,10 @@
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="7" t="s">
@@ -3640,8 +3671,8 @@
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
       <c r="E42" s="7" t="s">
         <v>5</v>
       </c>
@@ -3653,8 +3684,8 @@
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C43" s="21"/>
-      <c r="D43" s="20" t="s">
+      <c r="C43" s="22"/>
+      <c r="D43" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E43" s="7" t="s">
@@ -3668,8 +3699,8 @@
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="7" t="s">
         <v>5</v>
       </c>
@@ -3682,27 +3713,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C41:C44"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D21:D22"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:D6"/>
@@ -3713,6 +3723,27 @@
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="D15:D16"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C41:C44"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D37:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3736,13 +3767,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D5" s="12" t="s">
@@ -3762,10 +3793,10 @@
       </c>
     </row>
     <row r="6" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="13" t="s">
@@ -3779,8 +3810,8 @@
       </c>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="13" t="s">
         <v>5</v>
       </c>
@@ -3792,8 +3823,8 @@
       </c>
     </row>
     <row r="8" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D8" s="21"/>
-      <c r="E8" s="20" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="13" t="s">
@@ -3807,8 +3838,8 @@
       </c>
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="13" t="s">
         <v>5</v>
       </c>
@@ -3820,10 +3851,10 @@
       </c>
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="13" t="s">
@@ -3837,8 +3868,8 @@
       </c>
     </row>
     <row r="11" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="13" t="s">
         <v>5</v>
       </c>
@@ -3850,8 +3881,8 @@
       </c>
     </row>
     <row r="12" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D12" s="21"/>
-      <c r="E12" s="20" t="s">
+      <c r="D12" s="22"/>
+      <c r="E12" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="13" t="s">
@@ -3865,8 +3896,8 @@
       </c>
     </row>
     <row r="13" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
       <c r="F13" s="13" t="s">
         <v>5</v>
       </c>
@@ -3878,10 +3909,10 @@
       </c>
     </row>
     <row r="14" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="26" t="s">
         <v>3</v>
       </c>
       <c r="F14" s="13" t="s">
@@ -3895,8 +3926,8 @@
       </c>
     </row>
     <row r="15" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D15" s="21"/>
-      <c r="E15" s="19"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="25"/>
       <c r="F15" s="13" t="s">
         <v>5</v>
       </c>
@@ -3908,8 +3939,8 @@
       </c>
     </row>
     <row r="16" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D16" s="21"/>
-      <c r="E16" s="23" t="s">
+      <c r="D16" s="22"/>
+      <c r="E16" s="26" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="13" t="s">
@@ -3923,8 +3954,8 @@
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D17" s="21"/>
-      <c r="E17" s="19"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="25"/>
       <c r="F17" s="13" t="s">
         <v>5</v>
       </c>
@@ -3936,10 +3967,10 @@
       </c>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="26" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="13" t="s">
@@ -3953,8 +3984,8 @@
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D19" s="21"/>
-      <c r="E19" s="19"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="25"/>
       <c r="F19" s="13" t="s">
         <v>5</v>
       </c>
@@ -3966,8 +3997,8 @@
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D20" s="21"/>
-      <c r="E20" s="23" t="s">
+      <c r="D20" s="22"/>
+      <c r="E20" s="26" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="13" t="s">
@@ -3981,8 +4012,8 @@
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D21" s="21"/>
-      <c r="E21" s="19"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="25"/>
       <c r="F21" s="13" t="s">
         <v>5</v>
       </c>
@@ -3994,10 +4025,10 @@
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="13" t="s">
@@ -4011,8 +4042,8 @@
       </c>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
       <c r="F23" s="13" t="s">
         <v>5</v>
       </c>
@@ -4024,8 +4055,8 @@
       </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D24" s="21"/>
-      <c r="E24" s="20" t="s">
+      <c r="D24" s="22"/>
+      <c r="E24" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="13" t="s">
@@ -4039,8 +4070,8 @@
       </c>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="13" t="s">
         <v>5</v>
       </c>
@@ -4052,10 +4083,10 @@
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F26" s="13" t="s">
@@ -4069,8 +4100,8 @@
       </c>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="13" t="s">
         <v>5</v>
       </c>
@@ -4082,8 +4113,8 @@
       </c>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D28" s="21"/>
-      <c r="E28" s="20" t="s">
+      <c r="D28" s="22"/>
+      <c r="E28" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F28" s="13" t="s">
@@ -4097,8 +4128,8 @@
       </c>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
       <c r="F29" s="13" t="s">
         <v>5</v>
       </c>
@@ -4111,6 +4142,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="E6:E7"/>
@@ -4118,18 +4161,6 @@
     <mergeCell ref="D10:D13"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E28:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4153,13 +4184,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D5" s="14" t="s">
@@ -4179,10 +4210,10 @@
       </c>
     </row>
     <row r="6" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="15" t="s">
@@ -4196,8 +4227,8 @@
       </c>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="15" t="s">
         <v>5</v>
       </c>
@@ -4209,8 +4240,8 @@
       </c>
     </row>
     <row r="8" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D8" s="21"/>
-      <c r="E8" s="20" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="15" t="s">
@@ -4224,8 +4255,8 @@
       </c>
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="15" t="s">
         <v>5</v>
       </c>
@@ -4237,10 +4268,10 @@
       </c>
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="15" t="s">
@@ -4254,8 +4285,8 @@
       </c>
     </row>
     <row r="11" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="15" t="s">
         <v>5</v>
       </c>
@@ -4267,8 +4298,8 @@
       </c>
     </row>
     <row r="12" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D12" s="21"/>
-      <c r="E12" s="20" t="s">
+      <c r="D12" s="22"/>
+      <c r="E12" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="15" t="s">
@@ -4282,8 +4313,8 @@
       </c>
     </row>
     <row r="13" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
       <c r="F13" s="15" t="s">
         <v>5</v>
       </c>
@@ -4295,10 +4326,10 @@
       </c>
     </row>
     <row r="14" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="26" t="s">
         <v>3</v>
       </c>
       <c r="F14" s="15" t="s">
@@ -4312,8 +4343,8 @@
       </c>
     </row>
     <row r="15" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D15" s="21"/>
-      <c r="E15" s="19"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="25"/>
       <c r="F15" s="15" t="s">
         <v>5</v>
       </c>
@@ -4325,8 +4356,8 @@
       </c>
     </row>
     <row r="16" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D16" s="21"/>
-      <c r="E16" s="23" t="s">
+      <c r="D16" s="22"/>
+      <c r="E16" s="26" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="15" t="s">
@@ -4340,8 +4371,8 @@
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D17" s="21"/>
-      <c r="E17" s="19"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="25"/>
       <c r="F17" s="15" t="s">
         <v>5</v>
       </c>
@@ -4353,10 +4384,10 @@
       </c>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="15" t="s">
@@ -4370,8 +4401,8 @@
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
       <c r="F19" s="15" t="s">
         <v>5</v>
       </c>
@@ -4383,8 +4414,8 @@
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D20" s="21"/>
-      <c r="E20" s="20" t="s">
+      <c r="D20" s="22"/>
+      <c r="E20" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="15" t="s">
@@ -4398,8 +4429,8 @@
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="15" t="s">
         <v>5</v>
       </c>
@@ -4411,35 +4442,42 @@
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D26" s="22"/>
-      <c r="E26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D28" s="21"/>
-      <c r="E28" s="20"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
     <mergeCell ref="D26:D29"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="E28:E29"/>
@@ -4449,13 +4487,6 @@
     <mergeCell ref="D18:D21"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="E20:E21"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4466,8 +4497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E5A01A-9D4D-734D-9616-8CB061676FDB}">
   <dimension ref="D4:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4480,13 +4511,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D5" s="16" t="s">
@@ -4506,10 +4537,10 @@
       </c>
     </row>
     <row r="6" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="17" t="s">
@@ -4523,8 +4554,8 @@
       </c>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="17" t="s">
         <v>5</v>
       </c>
@@ -4536,8 +4567,8 @@
       </c>
     </row>
     <row r="8" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D8" s="21"/>
-      <c r="E8" s="20" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="17" t="s">
@@ -4551,8 +4582,8 @@
       </c>
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="17" t="s">
         <v>5</v>
       </c>
@@ -4564,10 +4595,10 @@
       </c>
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="17" t="s">
@@ -4581,8 +4612,8 @@
       </c>
     </row>
     <row r="11" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="17" t="s">
         <v>5</v>
       </c>
@@ -4594,8 +4625,8 @@
       </c>
     </row>
     <row r="12" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D12" s="21"/>
-      <c r="E12" s="20" t="s">
+      <c r="D12" s="22"/>
+      <c r="E12" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="17" t="s">
@@ -4609,8 +4640,8 @@
       </c>
     </row>
     <row r="13" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
       <c r="F13" s="17" t="s">
         <v>5</v>
       </c>
@@ -4622,10 +4653,10 @@
       </c>
     </row>
     <row r="14" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="26" t="s">
         <v>3</v>
       </c>
       <c r="F14" s="17" t="s">
@@ -4639,8 +4670,8 @@
       </c>
     </row>
     <row r="15" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D15" s="21"/>
-      <c r="E15" s="19"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="25"/>
       <c r="F15" s="17" t="s">
         <v>5</v>
       </c>
@@ -4652,8 +4683,8 @@
       </c>
     </row>
     <row r="16" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D16" s="21"/>
-      <c r="E16" s="23" t="s">
+      <c r="D16" s="22"/>
+      <c r="E16" s="26" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="17" t="s">
@@ -4667,8 +4698,8 @@
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D17" s="21"/>
-      <c r="E17" s="19"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="25"/>
       <c r="F17" s="17" t="s">
         <v>5</v>
       </c>
@@ -4680,10 +4711,10 @@
       </c>
     </row>
     <row r="18" spans="4:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="17" t="s">
@@ -4697,8 +4728,8 @@
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
       <c r="F19" s="17" t="s">
         <v>5</v>
       </c>
@@ -4710,8 +4741,8 @@
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D20" s="21"/>
-      <c r="E20" s="20" t="s">
+      <c r="D20" s="22"/>
+      <c r="E20" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="17" t="s">
@@ -4725,8 +4756,8 @@
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="17" t="s">
         <v>5</v>
       </c>
@@ -4738,41 +4769,35 @@
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D26" s="22"/>
-      <c r="E26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D28" s="21"/>
-      <c r="E28" s="20"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23"/>
       <c r="F28" s="17"/>
       <c r="G28" s="17"/>
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E28:E29"/>
     <mergeCell ref="D14:D17"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="E16:E17"/>
@@ -4783,6 +4808,12 @@
     <mergeCell ref="D10:D13"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E28:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4806,13 +4837,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D5" s="16" t="s">
@@ -4832,10 +4863,10 @@
       </c>
     </row>
     <row r="6" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="17" t="s">
@@ -4849,8 +4880,8 @@
       </c>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="17" t="s">
         <v>5</v>
       </c>
@@ -4862,8 +4893,8 @@
       </c>
     </row>
     <row r="8" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D8" s="21"/>
-      <c r="E8" s="20" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="17" t="s">
@@ -4877,8 +4908,8 @@
       </c>
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="17" t="s">
         <v>5</v>
       </c>
@@ -4890,10 +4921,10 @@
       </c>
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="17" t="s">
@@ -4907,8 +4938,8 @@
       </c>
     </row>
     <row r="11" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="17" t="s">
         <v>5</v>
       </c>
@@ -4920,8 +4951,8 @@
       </c>
     </row>
     <row r="12" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D12" s="21"/>
-      <c r="E12" s="20" t="s">
+      <c r="D12" s="22"/>
+      <c r="E12" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="17" t="s">
@@ -4935,8 +4966,8 @@
       </c>
     </row>
     <row r="13" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
       <c r="F13" s="17" t="s">
         <v>5</v>
       </c>
@@ -4948,10 +4979,10 @@
       </c>
     </row>
     <row r="14" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F14" s="17" t="s">
@@ -4965,8 +4996,8 @@
       </c>
     </row>
     <row r="15" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
       <c r="F15" s="17" t="s">
         <v>5</v>
       </c>
@@ -4978,8 +5009,8 @@
       </c>
     </row>
     <row r="16" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D16" s="21"/>
-      <c r="E16" s="20" t="s">
+      <c r="D16" s="22"/>
+      <c r="E16" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="17" t="s">
@@ -4993,8 +5024,8 @@
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
       <c r="F17" s="17" t="s">
         <v>5</v>
       </c>
@@ -5006,10 +5037,10 @@
       </c>
     </row>
     <row r="18" spans="4:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="26" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="17" t="s">
@@ -5023,8 +5054,8 @@
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D19" s="21"/>
-      <c r="E19" s="19"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="25"/>
       <c r="F19" s="17" t="s">
         <v>5</v>
       </c>
@@ -5036,8 +5067,8 @@
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D20" s="21"/>
-      <c r="E20" s="23" t="s">
+      <c r="D20" s="22"/>
+      <c r="E20" s="26" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="17" t="s">
@@ -5051,8 +5082,8 @@
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D21" s="21"/>
-      <c r="E21" s="19"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="25"/>
       <c r="F21" s="17" t="s">
         <v>5</v>
       </c>
@@ -5064,10 +5095,10 @@
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="17" t="s">
@@ -5081,8 +5112,8 @@
       </c>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
       <c r="F23" s="17" t="s">
         <v>5</v>
       </c>
@@ -5094,8 +5125,8 @@
       </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D24" s="21"/>
-      <c r="E24" s="20" t="s">
+      <c r="D24" s="22"/>
+      <c r="E24" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="17" t="s">
@@ -5109,8 +5140,8 @@
       </c>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="17" t="s">
         <v>5</v>
       </c>
@@ -5122,35 +5153,42 @@
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D26" s="22"/>
-      <c r="E26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D28" s="21"/>
-      <c r="E28" s="20"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23"/>
       <c r="F28" s="17"/>
       <c r="G28" s="17"/>
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
     <mergeCell ref="D26:D29"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="E28:E29"/>
@@ -5163,13 +5201,301 @@
     <mergeCell ref="D22:D25"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2256552-9452-4E44-AF56-A68E27D5D22A}">
+  <dimension ref="D5:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D5" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="19">
+        <v>0.98</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="19">
+        <v>0.98</v>
+      </c>
+      <c r="H8" s="19">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D9" s="22"/>
+      <c r="E9" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="19">
+        <v>0.69</v>
+      </c>
+      <c r="H9" s="19">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.96</v>
+      </c>
+      <c r="H11" s="20">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="20">
+        <v>0.92</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D13" s="22"/>
+      <c r="E13" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="20">
+        <v>0.71</v>
+      </c>
+      <c r="H13" s="20">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="20">
+        <v>0.95</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="20">
+        <v>0.92</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D17" s="22"/>
+      <c r="E17" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="20">
+        <v>0.71</v>
+      </c>
+      <c r="H17" s="20">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D19" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="20">
+        <v>0.96</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="20">
+        <v>0.92</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D21" s="22"/>
+      <c r="E21" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="20">
+        <v>0.71</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>